<commit_message>
add 8 and modifed 7
</commit_message>
<xml_diff>
--- a/7/7.xlsx
+++ b/7/7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Universidad\Base De Datos I\Ejercicios\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1037A9B2-D703-434D-B778-AD23228499CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC789E-0B17-4E86-B9CF-C7F93A086474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41F5236A-1FB0-44E4-8E22-10547072F9FE}"/>
   </bookViews>
@@ -381,18 +381,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -433,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -455,11 +449,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4087F089-D38C-4D77-ABFC-6251F8763106}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,22 +849,23 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -916,22 +912,23 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="13">
         <v>123456</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="13">
         <v>7654321</v>
       </c>
-      <c r="E4" s="2">
+      <c r="D4" s="14"/>
+      <c r="E4" s="12">
         <v>101</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="16">
         <v>45792</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="13">
         <v>123456</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -976,22 +973,23 @@
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="13">
         <v>765432</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="13">
         <v>7123456</v>
       </c>
-      <c r="E5" s="2">
+      <c r="D5" s="14"/>
+      <c r="E5" s="12">
         <v>102</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="16">
         <v>45792</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="13">
         <v>765432</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -1038,22 +1036,23 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="13">
         <v>234576</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="13">
         <v>7890123</v>
       </c>
-      <c r="E6" s="2">
+      <c r="D6" s="14"/>
+      <c r="E6" s="12">
         <v>103</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="16">
         <v>45793</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="13">
         <v>982378</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -1100,19 +1099,20 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="13">
         <v>982378</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="13">
         <v>6218931</v>
       </c>
-      <c r="E7" s="14">
+      <c r="D7" s="14"/>
+      <c r="E7" s="12">
         <v>104</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="16">
         <v>45793</v>
       </c>
       <c r="G7" s="13">
@@ -1124,19 +1124,20 @@
       <c r="I7" s="13">
         <v>478218</v>
       </c>
-      <c r="K7" s="2">
+      <c r="J7" s="14"/>
+      <c r="K7" s="12">
         <v>103</v>
       </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="L7" s="12">
+        <v>1</v>
+      </c>
+      <c r="M7" s="12">
+        <v>1</v>
+      </c>
+      <c r="N7" s="12">
         <v>42</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="12" t="s">
         <v>74</v>
       </c>
       <c r="Q7" s="2" t="s">
@@ -1160,19 +1161,20 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="13">
         <v>328130</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="13">
         <v>7832192</v>
       </c>
-      <c r="E8" s="14">
+      <c r="D8" s="14"/>
+      <c r="E8" s="12">
         <v>105</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="16">
         <v>45793</v>
       </c>
       <c r="G8" s="13">
@@ -1184,19 +1186,20 @@
       <c r="I8" s="13">
         <v>478218</v>
       </c>
-      <c r="K8" s="14">
+      <c r="J8" s="14"/>
+      <c r="K8" s="12">
         <v>104</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="12">
         <v>4</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="12">
         <v>6</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="12">
         <v>1.5</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="12" t="s">
         <v>53</v>
       </c>
       <c r="Q8" s="2" t="s">
@@ -1231,34 +1234,36 @@
       <c r="C9" s="13">
         <v>7112233</v>
       </c>
-      <c r="E9" s="2">
+      <c r="D9" s="14"/>
+      <c r="E9" s="12">
         <v>106</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="16">
         <v>45793</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="13">
         <v>982378</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="13">
         <v>982378</v>
       </c>
-      <c r="K9" s="14">
+      <c r="J9" s="14"/>
+      <c r="K9" s="12">
         <v>104</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="12">
         <v>4</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="12">
         <v>4</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="12">
         <v>4.5</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="O9" s="12" t="s">
         <v>55</v>
       </c>
       <c r="Q9" s="2" t="s">
@@ -1284,22 +1289,23 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="13">
         <v>671872</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="13">
         <v>7567892</v>
       </c>
-      <c r="E10" s="2">
+      <c r="D10" s="14"/>
+      <c r="E10" s="12">
         <v>107</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="16">
         <v>45794</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="13">
         <v>328130</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -1344,22 +1350,23 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="13">
         <v>298391</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="13">
         <v>7788992</v>
       </c>
-      <c r="E11" s="2">
+      <c r="D11" s="14"/>
+      <c r="E11" s="12">
         <v>108</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="16">
         <v>45794</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="13">
         <v>671872</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1406,13 +1413,17 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="E12" s="2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="12">
         <v>109</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="16">
         <v>45794</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="13">
         <v>298391</v>
       </c>
       <c r="H12" s="5" t="s">
@@ -1459,16 +1470,19 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="12">
         <v>110</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="16">
         <v>45795</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="13">
         <v>765432</v>
       </c>
       <c r="H13" s="5" t="s">

</xml_diff>

<commit_message>
fixed exercises and diagrams and tables
</commit_message>
<xml_diff>
--- a/7/7.xlsx
+++ b/7/7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Universidad\Base De Datos I\Ejercicios\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC789E-0B17-4E86-B9CF-C7F93A086474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B4D67B-DCE6-4CE8-861A-6C7F1E9A8417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41F5236A-1FB0-44E4-8E22-10547072F9FE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
   <si>
     <t>PK</t>
   </si>
@@ -341,13 +341,34 @@
   </si>
   <si>
     <t>DETALLEFACTURA</t>
+  </si>
+  <si>
+    <t>MONTOTOTAL</t>
+  </si>
+  <si>
+    <t>21.5</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>95.5</t>
+  </si>
+  <si>
+    <t>NRO</t>
+  </si>
+  <si>
+    <t>LA TABLA PRODUCTO Y LA TABLA CATEGORIA LA CAMBIO EL INGENIERO</t>
+  </si>
+  <si>
+    <t>POR LO TANTO QUEDA PENDIENTE ACTUALIZAR LAS CONSULTAS EN SQL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +397,16 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -455,6 +486,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4087F089-D38C-4D77-ABFC-6251F8763106}">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:U25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,72 +818,73 @@
     <col min="4" max="4" width="4.88671875" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
-    <col min="15" max="15" width="13.21875" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" customWidth="1"/>
-    <col min="17" max="17" width="8.44140625" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" customWidth="1"/>
-    <col min="20" max="20" width="7.109375" customWidth="1"/>
-    <col min="21" max="21" width="6.44140625" customWidth="1"/>
-    <col min="22" max="22" width="5.77734375" customWidth="1"/>
-    <col min="23" max="23" width="22.88671875" customWidth="1"/>
-    <col min="24" max="24" width="6.77734375" customWidth="1"/>
-    <col min="25" max="25" width="7.6640625" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" customWidth="1"/>
+    <col min="16" max="16" width="13.21875" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" customWidth="1"/>
+    <col min="18" max="18" width="8.44140625" customWidth="1"/>
+    <col min="19" max="19" width="18.109375" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" customWidth="1"/>
+    <col min="22" max="22" width="3.21875" customWidth="1"/>
+    <col min="23" max="23" width="11.77734375" customWidth="1"/>
+    <col min="24" max="24" width="22.88671875" customWidth="1"/>
+    <col min="25" max="25" width="6.77734375" customWidth="1"/>
+    <col min="26" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>102</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>0</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>9</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>0</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -860,7 +896,7 @@
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="15" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>7</v>
@@ -871,47 +907,50 @@
       <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>123456</v>
       </c>
@@ -934,45 +973,48 @@
       <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="7">
         <v>123456</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>101</v>
       </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
       <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>5</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="11">
+      <c r="T4" s="11">
         <v>2</v>
       </c>
-      <c r="T4" s="2">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
-      <c r="W4" s="2" t="s">
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>765432</v>
       </c>
@@ -995,47 +1037,50 @@
       <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="18">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5">
         <v>765432</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>101</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>4</v>
       </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
       <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
         <v>11.5</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>3</v>
       </c>
-      <c r="T5" s="2">
-        <v>1</v>
-      </c>
-      <c r="V5" s="2">
+      <c r="U5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2">
         <v>2</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>234576</v>
       </c>
@@ -1058,47 +1103,50 @@
       <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="18">
+        <v>42</v>
+      </c>
+      <c r="J6" s="5">
         <v>982378</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>102</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>12</v>
       </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
       <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2">
         <v>15</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>5</v>
       </c>
-      <c r="T6" s="2">
-        <v>1</v>
-      </c>
-      <c r="V6" s="2">
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2">
         <v>3</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="X6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>982378</v>
       </c>
@@ -1121,46 +1169,49 @@
       <c r="H7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="18">
+        <v>27</v>
+      </c>
+      <c r="J7" s="13">
         <v>478218</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12">
+      <c r="K7" s="14"/>
+      <c r="L7" s="12">
         <v>103</v>
       </c>
-      <c r="L7" s="12">
-        <v>1</v>
-      </c>
       <c r="M7" s="12">
         <v>1</v>
       </c>
       <c r="N7" s="12">
+        <v>1</v>
+      </c>
+      <c r="O7" s="12">
         <v>42</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>11</v>
       </c>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2">
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
         <v>4</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>328130</v>
       </c>
@@ -1183,48 +1234,51 @@
       <c r="H8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="18">
+        <v>183</v>
+      </c>
+      <c r="J8" s="13">
         <v>478218</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12">
+      <c r="K8" s="14"/>
+      <c r="L8" s="12">
         <v>104</v>
       </c>
-      <c r="L8" s="12">
+      <c r="M8" s="12">
         <v>4</v>
       </c>
-      <c r="M8" s="12">
+      <c r="N8" s="12">
         <v>6</v>
       </c>
-      <c r="N8" s="12">
+      <c r="O8" s="12">
         <v>1.5</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <v>42</v>
       </c>
-      <c r="T8" s="2">
-        <v>1</v>
-      </c>
-      <c r="V8" s="2">
+      <c r="U8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
         <v>5</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Y8" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>478218</v>
       </c>
@@ -1247,48 +1301,51 @@
       <c r="H9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="18">
+        <v>19</v>
+      </c>
+      <c r="J9" s="13">
         <v>982378</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12">
+      <c r="K9" s="14"/>
+      <c r="L9" s="12">
         <v>104</v>
-      </c>
-      <c r="L9" s="12">
-        <v>4</v>
       </c>
       <c r="M9" s="12">
         <v>4</v>
       </c>
       <c r="N9" s="12">
+        <v>4</v>
+      </c>
+      <c r="O9" s="12">
         <v>4.5</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="P9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>51</v>
       </c>
-      <c r="T9" s="2">
-        <v>1</v>
-      </c>
-      <c r="V9" s="2">
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2">
         <v>6</v>
       </c>
-      <c r="W9" s="9" t="s">
+      <c r="X9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Y9" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>671872</v>
       </c>
@@ -1311,45 +1368,48 @@
       <c r="H10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="18">
+        <v>50</v>
+      </c>
+      <c r="J10" s="5">
         <v>328130</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>105</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>4</v>
       </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
       <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
         <v>183</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S10" s="11">
+      <c r="T10" s="11">
         <v>1.5</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>4</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>7</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="X10" s="2"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y10" s="2"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>298391</v>
       </c>
@@ -1372,47 +1432,50 @@
       <c r="H11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="18">
+        <v>211</v>
+      </c>
+      <c r="J11" s="5">
         <v>671872</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>106</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>18</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>5</v>
       </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S11" s="11">
+      <c r="T11" s="11">
         <v>11.5</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>4</v>
       </c>
-      <c r="V11" s="2">
+      <c r="W11" s="2">
         <v>8</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Y11" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1429,47 +1492,50 @@
       <c r="H12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12" s="5">
         <v>298391</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>106</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>12</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>2</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>7</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="S12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>4.5</v>
       </c>
-      <c r="T12" s="2">
+      <c r="U12" s="2">
         <v>4</v>
       </c>
-      <c r="V12" s="2">
+      <c r="W12" s="2">
         <v>9</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="X12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="X12" s="2">
+      <c r="Y12" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14">
         <v>1</v>
@@ -1488,47 +1554,50 @@
       <c r="H13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="18">
+        <v>2</v>
+      </c>
+      <c r="J13" s="5">
         <v>765432</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>107</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>7</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>3</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>50</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S13" s="11">
+      <c r="T13" s="11">
         <v>54</v>
       </c>
-      <c r="T13" s="11">
+      <c r="U13" s="11">
         <v>4</v>
       </c>
-      <c r="V13" s="2">
+      <c r="W13" s="2">
         <v>10</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X13" s="2">
+      <c r="Y13" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E14" s="2">
         <v>111</v>
       </c>
@@ -1541,47 +1610,50 @@
       <c r="H14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="5">
         <v>671872</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>108</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>4</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>6</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>11.5</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="R14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <v>42</v>
       </c>
-      <c r="T14" s="2">
+      <c r="U14" s="2">
         <v>4</v>
       </c>
-      <c r="V14" s="2">
+      <c r="W14" s="2">
         <v>11</v>
       </c>
-      <c r="W14" s="9" t="s">
+      <c r="X14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="X14" s="2">
+      <c r="Y14" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E15" s="2">
         <v>112</v>
       </c>
@@ -1594,414 +1666,425 @@
       <c r="H15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="18">
+        <v>66</v>
+      </c>
+      <c r="J15" s="5">
         <v>328130</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>108</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>7</v>
       </c>
-      <c r="M15" s="2">
-        <v>1</v>
-      </c>
       <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
         <v>142</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="S15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S15" s="2">
+      <c r="T15" s="2">
         <v>183</v>
       </c>
-      <c r="T15" s="2">
+      <c r="U15" s="2">
         <v>4</v>
       </c>
-      <c r="V15" s="2">
+      <c r="W15" s="2">
         <v>12</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="X15" s="2"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="K16" s="12">
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="L16" s="12">
         <v>109</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>18</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>3</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>0.7</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="R16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="S16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S16" s="11">
+      <c r="T16" s="11">
         <v>142</v>
       </c>
-      <c r="T16" s="11">
+      <c r="U16" s="11">
         <v>7</v>
       </c>
-      <c r="V16" s="2">
+      <c r="W16" s="2">
         <v>13</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X16" s="2">
+      <c r="Y16" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F17">
         <v>2</v>
       </c>
-      <c r="K17" s="12">
+      <c r="L17" s="12">
         <v>110</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>18</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>2</v>
       </c>
-      <c r="N17" s="2">
-        <v>1</v>
-      </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="R17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="S17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S17" s="11">
+      <c r="T17" s="11">
         <v>89</v>
       </c>
-      <c r="T17" s="11">
+      <c r="U17" s="11">
         <v>7</v>
       </c>
-      <c r="V17" s="2">
+      <c r="W17" s="2">
         <v>14</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="X17" s="2">
+      <c r="Y17" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="K18" s="12">
+    <row r="18" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="L18" s="12">
         <v>111</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>15</v>
       </c>
-      <c r="M18" s="2">
-        <v>1</v>
-      </c>
       <c r="N18" s="2">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2">
         <v>75.5</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S18" s="2">
+      <c r="T18" s="2">
         <v>162</v>
       </c>
-      <c r="T18" s="2">
+      <c r="U18" s="2">
         <v>7</v>
       </c>
-      <c r="V18" s="2">
+      <c r="W18" s="2">
         <v>15</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="X18" s="2"/>
-    </row>
-    <row r="19" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="6:26" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
-      <c r="K19" s="12">
+      <c r="L19" s="12">
         <v>111</v>
       </c>
-      <c r="L19" s="2">
-        <v>1</v>
-      </c>
       <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
         <v>10</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <v>2</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="R19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S19" s="11">
+      <c r="T19" s="11">
         <v>50</v>
       </c>
-      <c r="T19" s="11">
+      <c r="U19" s="11">
         <v>7</v>
       </c>
-      <c r="V19" s="2">
+      <c r="W19" s="2">
         <v>16</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="X19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="X19" s="2">
+      <c r="Y19" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:26" x14ac:dyDescent="0.3">
       <c r="H20" s="8"/>
-      <c r="K20" s="12">
+      <c r="I20" s="8"/>
+      <c r="L20" s="12">
         <v>112</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>12</v>
       </c>
-      <c r="M20" s="2">
-        <v>1</v>
-      </c>
       <c r="N20" s="2">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
         <v>66</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="P20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="R20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R20" s="2" t="s">
+      <c r="S20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="S20" s="11">
+      <c r="T20" s="11">
         <v>66</v>
       </c>
-      <c r="T20" s="11">
+      <c r="U20" s="11">
         <v>12</v>
       </c>
-      <c r="V20" s="2">
+      <c r="W20" s="2">
         <v>17</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="X20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X20" s="2">
+      <c r="Y20" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:26" x14ac:dyDescent="0.3">
       <c r="H21" s="8"/>
-      <c r="Q21" s="2" t="s">
+      <c r="I21" s="8"/>
+      <c r="R21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="S21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S21" s="11">
+      <c r="T21" s="11">
         <v>7</v>
       </c>
-      <c r="T21" s="11">
+      <c r="U21" s="11">
         <v>12</v>
       </c>
-      <c r="V21" s="2">
+      <c r="W21" s="2">
         <v>18</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="X21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="X21" s="2"/>
-    </row>
-    <row r="22" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="M22">
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="N22">
         <v>3</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="R22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="S22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S22" s="11">
+      <c r="T22" s="11">
         <v>15</v>
       </c>
-      <c r="T22" s="11">
+      <c r="U22" s="11">
         <v>12</v>
       </c>
-      <c r="V22" s="2">
+      <c r="W22" s="2">
         <v>19</v>
       </c>
-      <c r="W22" s="9" t="s">
+      <c r="X22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="X22" s="2">
+      <c r="Y22" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q23" s="2" t="s">
+    <row r="23" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="S23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S23" s="11">
+      <c r="T23" s="11">
         <v>39</v>
       </c>
-      <c r="T23" s="11">
+      <c r="U23" s="11">
         <v>12</v>
       </c>
-      <c r="V23" s="2">
+      <c r="W23" s="2">
         <v>20</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X23" s="2">
+      <c r="Y23" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q24" s="2" t="s">
+    <row r="24" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="S24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S24" s="11">
+      <c r="T24" s="11">
         <v>75.5</v>
       </c>
-      <c r="T24" s="11">
+      <c r="U24" s="11">
         <v>15</v>
       </c>
-      <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
-    </row>
-    <row r="25" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q25" s="2" t="s">
+      <c r="Z24" s="10"/>
+    </row>
+    <row r="25" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R25" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="R25" s="2" t="s">
+      <c r="S25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S25" s="11">
+      <c r="T25" s="11">
         <v>60</v>
       </c>
-      <c r="T25" s="11">
+      <c r="U25" s="11">
         <v>15</v>
       </c>
-      <c r="X25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q26" s="2" t="s">
+      <c r="Y25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="S26" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="S26" s="2">
+      <c r="T26" s="2">
         <v>158.80000000000001</v>
       </c>
-      <c r="T26" s="2">
+      <c r="U26" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q27" s="2" t="s">
+      <c r="W26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R27" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="S27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="S27" s="2">
+      <c r="T27" s="2">
         <v>40</v>
       </c>
-      <c r="T27" s="2">
+      <c r="U27" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q28" s="2" t="s">
+      <c r="W27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="R28" s="2" t="s">
+      <c r="S28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="S28" s="2">
-        <v>1</v>
-      </c>
       <c r="T28" s="2">
+        <v>1</v>
+      </c>
+      <c r="U28" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q29" s="2" t="s">
+    <row r="29" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R29" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="S29" s="2">
+      <c r="T29" s="2">
         <v>0.6</v>
       </c>
-      <c r="T29" s="2">
+      <c r="U29" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="Q30" s="2" t="s">
+    <row r="30" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="R30" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="R30" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="S30" s="2">
+      <c r="T30" s="2">
         <v>0.7</v>
       </c>
-      <c r="T30" s="2">
+      <c r="U30" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="S32">
+    <row r="32" spans="6:26" x14ac:dyDescent="0.3">
+      <c r="T32">
         <v>2</v>
       </c>
     </row>

</xml_diff>